<commit_message>
Con ajuste de control de pago
</commit_message>
<xml_diff>
--- a/controlFacturas/Facturas por pagar.xlsx
+++ b/controlFacturas/Facturas por pagar.xlsx
@@ -15,6 +15,7 @@
   <definedNames>
     <definedName function="false" hidden="true" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$C$1:$C$67</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">Hoja1!$C$1:$C$67</definedName>
+    <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase_0" vbProcedure="false">Hoja1!$C$1:$C$67</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -205,7 +206,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -244,10 +245,6 @@
     </xf>
     <xf numFmtId="164" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -357,16 +354,14 @@
   </sheetPr>
   <dimension ref="A1:N67"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D57" activeCellId="0" sqref="D57:D62"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E65" activeCellId="0" sqref="E65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="10.7773279352227"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.2267206477733"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="23.6315789473684"/>
-    <col collapsed="false" hidden="false" max="1025" min="6" style="0" width="10.7773279352227"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.4696356275304"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="24.1174089068826"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -683,10 +678,10 @@
       <c r="A21" s="3" t="n">
         <v>42499</v>
       </c>
-      <c r="B21" s="10" t="n">
+      <c r="B21" s="4" t="n">
         <v>171</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="4" t="n">
         <v>4510557708</v>
       </c>
       <c r="D21" s="5" t="n">
@@ -700,10 +695,10 @@
       <c r="A22" s="3" t="n">
         <v>42502</v>
       </c>
-      <c r="B22" s="10" t="n">
+      <c r="B22" s="4" t="n">
         <v>172</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="4" t="n">
         <v>4510555098</v>
       </c>
       <c r="D22" s="5" t="n">
@@ -717,10 +712,10 @@
       <c r="A23" s="3" t="n">
         <v>42510</v>
       </c>
-      <c r="B23" s="10" t="n">
+      <c r="B23" s="4" t="n">
         <v>173</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="4" t="n">
         <v>4510561570</v>
       </c>
       <c r="D23" s="5" t="n">
@@ -732,10 +727,10 @@
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
-      <c r="B24" s="10" t="n">
+      <c r="B24" s="4" t="n">
         <v>174</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="4" t="n">
         <v>4510563874</v>
       </c>
       <c r="D24" s="5" t="n">
@@ -749,10 +744,10 @@
       <c r="A25" s="3" t="n">
         <v>42514</v>
       </c>
-      <c r="B25" s="10" t="n">
+      <c r="B25" s="4" t="n">
         <v>175</v>
       </c>
-      <c r="C25" s="10" t="n">
+      <c r="C25" s="4" t="n">
         <v>4510568796</v>
       </c>
       <c r="D25" s="5" t="n">
@@ -764,7 +759,7 @@
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
-      <c r="B26" s="10" t="n">
+      <c r="B26" s="4" t="n">
         <v>176</v>
       </c>
       <c r="C26" s="4" t="s">
@@ -778,16 +773,16 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="11" t="n">
+      <c r="A27" s="10" t="n">
         <v>42530</v>
       </c>
-      <c r="B27" s="12" t="n">
+      <c r="B27" s="11" t="n">
         <v>177</v>
       </c>
-      <c r="C27" s="12" t="n">
+      <c r="C27" s="11" t="n">
         <v>4510568859</v>
       </c>
-      <c r="D27" s="13" t="n">
+      <c r="D27" s="12" t="n">
         <v>5000</v>
       </c>
       <c r="E27" s="6" t="n">
@@ -795,14 +790,14 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="11"/>
-      <c r="B28" s="12" t="n">
+      <c r="A28" s="10"/>
+      <c r="B28" s="11" t="n">
         <v>178</v>
       </c>
-      <c r="C28" s="12" t="n">
+      <c r="C28" s="11" t="n">
         <v>4510576584</v>
       </c>
-      <c r="D28" s="13" t="n">
+      <c r="D28" s="12" t="n">
         <v>76130</v>
       </c>
       <c r="E28" s="6" t="n">
@@ -811,17 +806,17 @@
       <c r="G28" s="0" t="n">
         <v>76891.3</v>
       </c>
-      <c r="N28" s="14"/>
+      <c r="N28" s="13"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="11"/>
-      <c r="B29" s="12" t="n">
+      <c r="A29" s="10"/>
+      <c r="B29" s="11" t="n">
         <v>179</v>
       </c>
-      <c r="C29" s="12" t="n">
+      <c r="C29" s="11" t="n">
         <v>4510577200</v>
       </c>
-      <c r="D29" s="13" t="n">
+      <c r="D29" s="12" t="n">
         <v>3400</v>
       </c>
       <c r="E29" s="6" t="n">
@@ -829,14 +824,14 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="11"/>
-      <c r="B30" s="12" t="n">
+      <c r="A30" s="10"/>
+      <c r="B30" s="11" t="n">
         <v>180</v>
       </c>
-      <c r="C30" s="12" t="n">
+      <c r="C30" s="11" t="n">
         <v>4510580329</v>
       </c>
-      <c r="D30" s="13" t="n">
+      <c r="D30" s="12" t="n">
         <v>3400</v>
       </c>
       <c r="E30" s="6" t="n">
@@ -847,7 +842,7 @@
       <c r="A31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B31" s="10" t="n">
+      <c r="B31" s="4" t="n">
         <v>181</v>
       </c>
       <c r="C31" s="4" t="s">
@@ -1245,9 +1240,11 @@
       <c r="D57" s="5" t="n">
         <v>16920</v>
       </c>
-      <c r="E57" s="6"/>
-    </row>
-    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="6" t="n">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="3"/>
       <c r="B58" s="4" t="n">
         <f aca="false">B57+1</f>
@@ -1259,9 +1256,11 @@
       <c r="D58" s="5" t="n">
         <v>12000</v>
       </c>
-      <c r="E58" s="6"/>
-    </row>
-    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="6" t="n">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="3"/>
       <c r="B59" s="4" t="n">
         <f aca="false">B58+1</f>
@@ -1273,9 +1272,11 @@
       <c r="D59" s="5" t="n">
         <v>52680</v>
       </c>
-      <c r="E59" s="6"/>
-    </row>
-    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="6" t="n">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="3"/>
       <c r="B60" s="4" t="n">
         <f aca="false">B59+1</f>
@@ -1287,9 +1288,11 @@
       <c r="D60" s="5" t="n">
         <v>87960</v>
       </c>
-      <c r="E60" s="6"/>
-    </row>
-    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="6" t="n">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="3"/>
       <c r="B61" s="4" t="n">
         <f aca="false">B60+1</f>
@@ -1301,9 +1304,11 @@
       <c r="D61" s="5" t="n">
         <v>4200</v>
       </c>
-      <c r="E61" s="6"/>
-    </row>
-    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E61" s="6" t="n">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="3"/>
       <c r="B62" s="4" t="n">
         <f aca="false">B61+1</f>
@@ -1315,7 +1320,9 @@
       <c r="D62" s="5" t="n">
         <v>50080</v>
       </c>
-      <c r="E62" s="6"/>
+      <c r="E62" s="6" t="n">
+        <v>42634</v>
+      </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="3"/>
@@ -1345,7 +1352,9 @@
       <c r="D64" s="5" t="n">
         <v>3000</v>
       </c>
-      <c r="E64" s="6"/>
+      <c r="E64" s="6" t="n">
+        <v>42634</v>
+      </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="3"/>
@@ -1362,12 +1371,12 @@
       <c r="E66" s="6"/>
     </row>
     <row r="67" customFormat="false" ht="21" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="15" t="s">
+      <c r="A67" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B67" s="15"/>
-      <c r="C67" s="15"/>
-      <c r="D67" s="16" t="n">
+      <c r="B67" s="14"/>
+      <c r="C67" s="14"/>
+      <c r="D67" s="15" t="n">
         <f aca="false">SUM(D3:D30)</f>
         <v>575290.82</v>
       </c>
@@ -1411,13 +1420,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D57:D62 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7773279352227"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -1437,13 +1443,10 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D57:D62 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="10.7773279352227"/>
-  </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>